<commit_message>
Finished adding the new raid.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Armour/specialty_armour.xlsx
+++ b/resources/data-imports/Armour/specialty_armour.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="196">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -563,6 +563,51 @@
   </si>
   <si>
     <t xml:space="preserve">plate sleeves that slowly leach the faith of those who ware them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shroud of the Sable Labyrinth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labyrinth Cloth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A heavy wrap of midnight cloth stitched with shifting maze-runes; in dim light its seams reroute like corridors, hiding the wearer among dead ends.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treadwraps of the Unending Turn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bandages of frayed velvet and iron-thread that drink sound; each step feels guided by an unseen path, yet the floor never remembers where you came from.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loombound Grips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Silken gloves woven on a cursed loom, patterned like tight passages; your fingers follow the thread-map, finding knots, locks, and hidden latches by instinct.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hood of the Hollow Junction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A layered cowl of dusky cloth veils the face behind intersecting folds; whispers run the pleats, warning of left turns that lead to nothing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weftwalker Leggings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quilted leggings of maze-tapestry, padded with cold ash; they move like hanging drapes, letting you slip through gaps where walls should close.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buckler of the Knotted Maze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A small buckler wrapped in spiral linens and bound with braided cords; blows sink into its woven circles, lost in a labyrinth of thread.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleeves of the Twisting Passage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Long sleeves of dark brocade, embroidered with endless corridors; when you lift your arms, the pattern shifts, confusing any eye that tries to measure your reach.</t>
   </si>
 </sst>
 </file>
@@ -612,7 +657,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -636,8 +681,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -646,14 +695,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -769,13 +827,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BS50"/>
+  <dimension ref="A1:BS57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44:J50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="35.66"/>
@@ -1080,9 +1138,7 @@
       <c r="G2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>2000000</v>
-      </c>
+      <c r="H2" s="0"/>
       <c r="J2" s="1" t="n">
         <v>2400000000</v>
       </c>
@@ -1458,9 +1514,7 @@
       <c r="G5" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H5" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="H5" s="0"/>
       <c r="J5" s="1" t="n">
         <v>3400000000</v>
       </c>
@@ -7044,6 +7098,1063 @@
       <c r="BP50" s="1" t="n">
         <v>0</v>
       </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H51" s="2"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="2" t="n">
+        <v>2400000000</v>
+      </c>
+      <c r="K51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S51" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="T51" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="U51" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="V51" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="W51" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="X51" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Y51" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
+      <c r="AB51" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC51" s="3"/>
+      <c r="AD51" s="3"/>
+      <c r="AE51" s="3"/>
+      <c r="AF51" s="3"/>
+      <c r="AG51" s="3"/>
+      <c r="AH51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM51" s="3"/>
+      <c r="AN51" s="3"/>
+      <c r="AO51" s="3"/>
+      <c r="AP51" s="3"/>
+      <c r="AQ51" s="3"/>
+      <c r="AR51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS51" s="3"/>
+      <c r="AT51" s="3"/>
+      <c r="AU51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV51" s="3"/>
+      <c r="AW51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY51" s="3"/>
+      <c r="AZ51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG51" s="3"/>
+      <c r="BH51" s="3"/>
+      <c r="BI51" s="3"/>
+      <c r="BJ51" s="3"/>
+      <c r="BK51" s="3"/>
+      <c r="BL51" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ51" s="3"/>
+      <c r="BR51" s="3"/>
+      <c r="BS51" s="3"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="2" t="n">
+        <v>2400000000</v>
+      </c>
+      <c r="K52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S52" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="T52" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="U52" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="V52" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="W52" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="X52" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Y52" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z52" s="3"/>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC52" s="3"/>
+      <c r="AD52" s="3"/>
+      <c r="AE52" s="3"/>
+      <c r="AF52" s="3"/>
+      <c r="AG52" s="3"/>
+      <c r="AH52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM52" s="3"/>
+      <c r="AN52" s="3"/>
+      <c r="AO52" s="3"/>
+      <c r="AP52" s="3"/>
+      <c r="AQ52" s="3"/>
+      <c r="AR52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS52" s="3"/>
+      <c r="AT52" s="3"/>
+      <c r="AU52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV52" s="3"/>
+      <c r="AW52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY52" s="3"/>
+      <c r="AZ52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG52" s="3"/>
+      <c r="BH52" s="3"/>
+      <c r="BI52" s="3"/>
+      <c r="BJ52" s="3"/>
+      <c r="BK52" s="3"/>
+      <c r="BL52" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP52" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ52" s="3"/>
+      <c r="BR52" s="3"/>
+      <c r="BS52" s="3"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D53" s="3"/>
+      <c r="E53" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="2" t="n">
+        <v>2400000000</v>
+      </c>
+      <c r="K53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S53" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="T53" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="U53" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="V53" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="W53" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="X53" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Y53" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z53" s="3"/>
+      <c r="AA53" s="3"/>
+      <c r="AB53" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC53" s="3"/>
+      <c r="AD53" s="3"/>
+      <c r="AE53" s="3"/>
+      <c r="AF53" s="3"/>
+      <c r="AG53" s="3"/>
+      <c r="AH53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM53" s="3"/>
+      <c r="AN53" s="3"/>
+      <c r="AO53" s="3"/>
+      <c r="AP53" s="3"/>
+      <c r="AQ53" s="3"/>
+      <c r="AR53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS53" s="3"/>
+      <c r="AT53" s="3"/>
+      <c r="AU53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV53" s="3"/>
+      <c r="AW53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY53" s="3"/>
+      <c r="AZ53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG53" s="3"/>
+      <c r="BH53" s="3"/>
+      <c r="BI53" s="3"/>
+      <c r="BJ53" s="3"/>
+      <c r="BK53" s="3"/>
+      <c r="BL53" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ53" s="3"/>
+      <c r="BR53" s="3"/>
+      <c r="BS53" s="3"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="2" t="n">
+        <v>2400000000</v>
+      </c>
+      <c r="K54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S54" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="T54" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="U54" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="V54" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="W54" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="X54" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Y54" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z54" s="3"/>
+      <c r="AA54" s="3"/>
+      <c r="AB54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC54" s="3"/>
+      <c r="AD54" s="3"/>
+      <c r="AE54" s="3"/>
+      <c r="AF54" s="3"/>
+      <c r="AG54" s="3"/>
+      <c r="AH54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM54" s="3"/>
+      <c r="AN54" s="3"/>
+      <c r="AO54" s="3"/>
+      <c r="AP54" s="3"/>
+      <c r="AQ54" s="3"/>
+      <c r="AR54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS54" s="3"/>
+      <c r="AT54" s="3"/>
+      <c r="AU54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV54" s="3"/>
+      <c r="AW54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY54" s="3"/>
+      <c r="AZ54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG54" s="3"/>
+      <c r="BH54" s="3"/>
+      <c r="BI54" s="3"/>
+      <c r="BJ54" s="3"/>
+      <c r="BK54" s="3"/>
+      <c r="BL54" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ54" s="3"/>
+      <c r="BR54" s="3"/>
+      <c r="BS54" s="3"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="2" t="n">
+        <v>2400000000</v>
+      </c>
+      <c r="K55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S55" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="T55" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="U55" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="V55" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="W55" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="X55" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Y55" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z55" s="3"/>
+      <c r="AA55" s="3"/>
+      <c r="AB55" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC55" s="3"/>
+      <c r="AD55" s="3"/>
+      <c r="AE55" s="3"/>
+      <c r="AF55" s="3"/>
+      <c r="AG55" s="3"/>
+      <c r="AH55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM55" s="3"/>
+      <c r="AN55" s="3"/>
+      <c r="AO55" s="3"/>
+      <c r="AP55" s="3"/>
+      <c r="AQ55" s="3"/>
+      <c r="AR55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS55" s="3"/>
+      <c r="AT55" s="3"/>
+      <c r="AU55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV55" s="3"/>
+      <c r="AW55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY55" s="3"/>
+      <c r="AZ55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG55" s="3"/>
+      <c r="BH55" s="3"/>
+      <c r="BI55" s="3"/>
+      <c r="BJ55" s="3"/>
+      <c r="BK55" s="3"/>
+      <c r="BL55" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ55" s="3"/>
+      <c r="BR55" s="3"/>
+      <c r="BS55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="2" t="n">
+        <v>2400000000</v>
+      </c>
+      <c r="K56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S56" s="3"/>
+      <c r="T56" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="U56" s="3"/>
+      <c r="V56" s="3"/>
+      <c r="W56" s="3"/>
+      <c r="X56" s="3"/>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3"/>
+      <c r="AA56" s="3"/>
+      <c r="AB56" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC56" s="3"/>
+      <c r="AD56" s="3"/>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="3"/>
+      <c r="AH56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM56" s="3"/>
+      <c r="AN56" s="3"/>
+      <c r="AO56" s="3"/>
+      <c r="AP56" s="3"/>
+      <c r="AQ56" s="3"/>
+      <c r="AR56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS56" s="3"/>
+      <c r="AT56" s="3"/>
+      <c r="AU56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV56" s="3"/>
+      <c r="AW56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY56" s="3"/>
+      <c r="AZ56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG56" s="3"/>
+      <c r="BH56" s="3"/>
+      <c r="BI56" s="3"/>
+      <c r="BJ56" s="3"/>
+      <c r="BK56" s="3"/>
+      <c r="BL56" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ56" s="3"/>
+      <c r="BR56" s="3"/>
+      <c r="BS56" s="3"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="2" t="n">
+        <v>2400000000</v>
+      </c>
+      <c r="K57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="S57" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="T57" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="U57" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="V57" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="W57" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="X57" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Y57" s="2" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="Z57" s="3"/>
+      <c r="AA57" s="3"/>
+      <c r="AB57" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC57" s="3"/>
+      <c r="AD57" s="3"/>
+      <c r="AE57" s="3"/>
+      <c r="AF57" s="3"/>
+      <c r="AG57" s="3"/>
+      <c r="AH57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM57" s="3"/>
+      <c r="AN57" s="3"/>
+      <c r="AO57" s="3"/>
+      <c r="AP57" s="3"/>
+      <c r="AQ57" s="3"/>
+      <c r="AR57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS57" s="3"/>
+      <c r="AT57" s="3"/>
+      <c r="AU57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV57" s="3"/>
+      <c r="AW57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY57" s="3"/>
+      <c r="AZ57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG57" s="3"/>
+      <c r="BH57" s="3"/>
+      <c r="BI57" s="3"/>
+      <c r="BJ57" s="3"/>
+      <c r="BK57" s="3"/>
+      <c r="BL57" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="BM57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP57" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ57" s="3"/>
+      <c r="BR57" s="3"/>
+      <c r="BS57" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>